<commit_message>
add feeding history to group and individual reports
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-feeding.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-feeding.xlsx
@@ -23,8 +23,148 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of the Tank</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Feeding method, matching feeding method in database, eg. Automatic</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional, frequency of feeding. Eg. Daily, Hourly, One Time</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Type of feed, must match Feed Code in database</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Size of feed, should be a number. Eg 0.5, 1, 2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Type of feed, must match Feed Code in database</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Size of feed, should be a number. Eg 0.5, 1, 2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Type of feed, must match Feed Code in database</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Size of feed, should be a number. Eg 0.5, 1, 2</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Tank</t>
   </si>
@@ -51,13 +191,19 @@
   </si>
   <si>
     <t>Feed Size 3</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Add extra feed columns if needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,16 +211,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,12 +240,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,56 +536,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>